<commit_message>
Change usage format to the same in Danube (capital letters without accent). Consider 'Commercial et services' == commerce, before it was equal to nan.
</commit_message>
<xml_diff>
--- a/DANUBE_preprocessing_tools/category_mapping/map_reference/associations_activ_nature_usage_danube.xlsx
+++ b/DANUBE_preprocessing_tools/category_mapping/map_reference/associations_activ_nature_usage_danube.xlsx
@@ -34,70 +34,70 @@
     <t xml:space="preserve">Aire d'accueil des gens du voyage</t>
   </si>
   <si>
-    <t xml:space="preserve">bâtiment agricole</t>
+    <t xml:space="preserve">BATIMENT AGRICOLE</t>
   </si>
   <si>
     <t xml:space="preserve">Autre service déconcentré de l'Etat</t>
   </si>
   <si>
-    <t xml:space="preserve">tertiaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bâtiment d'enseignement</t>
+    <t xml:space="preserve">TERTIAIRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATIMENT D ENSEIGNEMENT</t>
   </si>
   <si>
     <t xml:space="preserve">Borne</t>
   </si>
   <si>
-    <t xml:space="preserve">bâtiment industriel</t>
+    <t xml:space="preserve">BATIMENT INDUSTRIEL</t>
   </si>
   <si>
     <t xml:space="preserve">Borne frontière</t>
   </si>
   <si>
-    <t xml:space="preserve">bâtiment de santé</t>
+    <t xml:space="preserve">BATIMENT DE SANTE</t>
   </si>
   <si>
     <t xml:space="preserve">Camp militaire non clos</t>
   </si>
   <si>
-    <t xml:space="preserve">bâtiment religieux</t>
+    <t xml:space="preserve">BATIMENT RELIGIEUX</t>
   </si>
   <si>
     <t xml:space="preserve">Capitainerie</t>
   </si>
   <si>
-    <t xml:space="preserve">bâtiment sportif</t>
+    <t xml:space="preserve">BATIMENT SPORTIF</t>
   </si>
   <si>
     <t xml:space="preserve">Caserne</t>
   </si>
   <si>
-    <t xml:space="preserve">château</t>
+    <t xml:space="preserve">CHATEAU</t>
   </si>
   <si>
     <t xml:space="preserve">Caserne de pompiers</t>
   </si>
   <si>
-    <t xml:space="preserve">commerce</t>
+    <t xml:space="preserve">COMMERCE</t>
   </si>
   <si>
     <t xml:space="preserve">Divers public ou administratif</t>
   </si>
   <si>
-    <t xml:space="preserve">habitat</t>
+    <t xml:space="preserve">HABITAT</t>
   </si>
   <si>
     <t xml:space="preserve">Enceinte militaire</t>
   </si>
   <si>
-    <t xml:space="preserve">local non chauffé</t>
+    <t xml:space="preserve">LOCAL NON CHAUFFE</t>
   </si>
   <si>
     <t xml:space="preserve">Etablissement extraterritorial</t>
   </si>
   <si>
-    <t xml:space="preserve">serre agricole</t>
+    <t xml:space="preserve">SERRE AGRICOLE</t>
   </si>
   <si>
     <t xml:space="preserve">Etablissement pénitentiaire</t>
@@ -521,7 +521,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -599,14 +599,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -693,8 +685,8 @@
   </sheetPr>
   <dimension ref="A1:XFC100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B61" activeCellId="0" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1238,7 +1230,7 @@
       <c r="A65" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1246,7 +1238,7 @@
       <c r="A66" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1254,7 +1246,7 @@
       <c r="A67" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1262,7 +1254,7 @@
       <c r="A68" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1276,7 +1268,7 @@
       <c r="A70" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1284,7 +1276,7 @@
       <c r="A71" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1292,7 +1284,7 @@
       <c r="A72" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1477,7 +1469,7 @@
       <c r="B97" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="22" t="s">
+      <c r="A100" s="20" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>